<commit_message>
try to use gensim
</commit_message>
<xml_diff>
--- a/Excel/stop_count_df.xlsx
+++ b/Excel/stop_count_df.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icech\Desktop\share\Lab\2018_09_05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icech\Desktop\share\Lab\2018_09_05\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A9A7BA-19D0-4134-AE2D-5308D18E7018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8700354-C55A-4503-84F5-073E4ED50F19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34215" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34215" windowHeight="10800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="stop_count_df" sheetId="1" r:id="rId1"/>
@@ -2701,7 +2701,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -3667,25 +3667,25 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="21" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4045,7 +4045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="AN1" workbookViewId="0">
       <selection activeCell="AM20" sqref="AM20"/>
     </sheetView>
   </sheetViews>
@@ -31210,8 +31210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA5E9DC-D57E-4E92-B244-448CBAC2DCDB}">
   <dimension ref="A1:AO57"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AF27" sqref="AF27"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -32065,7 +32065,7 @@
         <v>132</v>
       </c>
       <c r="U18" s="14">
-        <f t="shared" si="0"/>
+        <f>IFERROR(VLOOKUP($T18,A$2:B$1000,2,0),"")</f>
         <v>14</v>
       </c>
       <c r="V18" s="15">
@@ -32308,7 +32308,7 @@
         <v>8</v>
       </c>
       <c r="AA21" t="str">
-        <f>IFERROR(VLOOKUP($T19,U$2:V$995,2,0),"")</f>
+        <f t="shared" ref="AA21:AA26" si="6">IFERROR(VLOOKUP($T19,U$2:V$995,2,0),"")</f>
         <v/>
       </c>
       <c r="AB21" s="30" t="s">
@@ -32390,7 +32390,7 @@
         <v>0</v>
       </c>
       <c r="AA22" t="str">
-        <f>IFERROR(VLOOKUP($T20,U$2:V$995,2,0),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB22" s="31">
@@ -32472,7 +32472,7 @@
         <v>0</v>
       </c>
       <c r="AA23" t="str">
-        <f>IFERROR(VLOOKUP($T21,U$2:V$995,2,0),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB23" t="str">
@@ -32545,7 +32545,7 @@
         <v>6</v>
       </c>
       <c r="AA24" t="str">
-        <f>IFERROR(VLOOKUP($T22,U$2:V$995,2,0),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB24" t="str">
@@ -32618,7 +32618,7 @@
         <v>12</v>
       </c>
       <c r="AA25" t="str">
-        <f>IFERROR(VLOOKUP($T23,U$2:V$995,2,0),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB25" t="str">
@@ -32667,31 +32667,31 @@
         <v>855</v>
       </c>
       <c r="U26" s="20">
-        <f>SUM(U17:U25)</f>
+        <f t="shared" ref="U26:Z26" si="7">SUM(U17:U25)</f>
         <v>542</v>
       </c>
       <c r="V26" s="21">
-        <f>SUM(V17:V25)</f>
+        <f t="shared" si="7"/>
         <v>500</v>
       </c>
       <c r="W26" s="21">
-        <f>SUM(W17:W25)</f>
+        <f t="shared" si="7"/>
         <v>575</v>
       </c>
       <c r="X26" s="21">
-        <f>SUM(X17:X25)</f>
+        <f t="shared" si="7"/>
         <v>534</v>
       </c>
       <c r="Y26" s="21">
-        <f>SUM(Y17:Y25)</f>
+        <f t="shared" si="7"/>
         <v>719</v>
       </c>
       <c r="Z26" s="22">
-        <f>SUM(Z17:Z25)</f>
+        <f t="shared" si="7"/>
         <v>368</v>
       </c>
       <c r="AA26" t="str">
-        <f>IFERROR(VLOOKUP($T24,U$2:V$995,2,0),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB26" t="str">
@@ -32832,7 +32832,7 @@
         <v>568</v>
       </c>
       <c r="Y29" s="12">
-        <f>IFERROR(VLOOKUP($T29,M$2:N$1000,2,0),"")</f>
+        <f t="shared" ref="Y29:Y35" si="8">IFERROR(VLOOKUP($T29,M$2:N$1000,2,0),"")</f>
         <v>808</v>
       </c>
       <c r="Z29" s="12">
@@ -32897,7 +32897,7 @@
         <v>23</v>
       </c>
       <c r="Y30" s="15">
-        <f>IFERROR(VLOOKUP($T30,M$2:N$1000,2,0),"")</f>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="Z30" s="15">
@@ -32967,7 +32967,7 @@
         <v>1</v>
       </c>
       <c r="Y31" s="15">
-        <f>IFERROR(VLOOKUP($T31,M$2:N$1000,2,0),"")</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Z31" s="14">
@@ -33039,7 +33039,7 @@
         <v>2</v>
       </c>
       <c r="Y32" s="15">
-        <f>IFERROR(VLOOKUP($T32,M$2:N$1000,2,0),"")</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="Z32" s="15">
@@ -33109,7 +33109,7 @@
         <v>0</v>
       </c>
       <c r="Y33" s="15">
-        <f>IFERROR(VLOOKUP($T33,M$2:N$1000,2,0),"")</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="Z33" s="14">
@@ -33181,7 +33181,7 @@
         <v>28</v>
       </c>
       <c r="Y34" s="15">
-        <f>IFERROR(VLOOKUP($T34,M$2:N$1000,2,0),"")</f>
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
       <c r="Z34" s="15">
@@ -33254,7 +33254,7 @@
         <v>13</v>
       </c>
       <c r="Y35" s="15">
-        <f>IFERROR(VLOOKUP($T35,M$2:N$1000,2,0),"")</f>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="Z35" s="15">
@@ -33311,27 +33311,27 @@
         <v>855</v>
       </c>
       <c r="U36" s="25">
-        <f>SUM(U29:U35)</f>
+        <f t="shared" ref="U36:Z36" si="9">SUM(U29:U35)</f>
         <v>673</v>
       </c>
       <c r="V36" s="25">
-        <f>SUM(V29:V35)</f>
+        <f t="shared" si="9"/>
         <v>604</v>
       </c>
       <c r="W36" s="25">
-        <f>SUM(W29:W35)</f>
+        <f t="shared" si="9"/>
         <v>663</v>
       </c>
       <c r="X36" s="25">
-        <f>SUM(X29:X35)</f>
+        <f t="shared" si="9"/>
         <v>635</v>
       </c>
       <c r="Y36" s="25">
-        <f>SUM(Y29:Y35)</f>
+        <f t="shared" si="9"/>
         <v>888</v>
       </c>
       <c r="Z36" s="26">
-        <f>SUM(Z29:Z35)</f>
+        <f t="shared" si="9"/>
         <v>473</v>
       </c>
       <c r="AA36" t="str">
@@ -33384,27 +33384,27 @@
         <v>857</v>
       </c>
       <c r="U37" s="28">
-        <f>U26/U36</f>
+        <f t="shared" ref="U37:Z37" si="10">U26/U36</f>
         <v>0.80534918276374445</v>
       </c>
       <c r="V37" s="28">
-        <f>V26/V36</f>
+        <f t="shared" si="10"/>
         <v>0.82781456953642385</v>
       </c>
       <c r="W37" s="28">
-        <f>W26/W36</f>
+        <f t="shared" si="10"/>
         <v>0.86726998491704377</v>
       </c>
       <c r="X37" s="28">
-        <f>X26/X36</f>
+        <f t="shared" si="10"/>
         <v>0.8409448818897638</v>
       </c>
       <c r="Y37" s="28">
-        <f>Y26/Y36</f>
+        <f t="shared" si="10"/>
         <v>0.80968468468468469</v>
       </c>
       <c r="Z37" s="29">
-        <f>Z26/Z36</f>
+        <f t="shared" si="10"/>
         <v>0.77801268498942922</v>
       </c>
       <c r="AA37" t="str">

</xml_diff>